<commit_message>
added 2 test cases
</commit_message>
<xml_diff>
--- a/office docs/Squad2 MVP1 UAT Sign-off_overall.xlsx
+++ b/office docs/Squad2 MVP1 UAT Sign-off_overall.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="538">
   <si>
     <t>#</t>
   </si>
@@ -628,7 +628,7 @@
     <t>LG mobile</t>
   </si>
   <si>
-    <t>Progress Status as of 2-2-2021</t>
+    <t>Progress Status as of 4-2-2021</t>
   </si>
   <si>
     <t>Project Name</t>
@@ -6004,10 +6004,319 @@
     <t>110</t>
   </si>
   <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Company Information Section</t>
+  </si>
+  <si>
+    <t>1.a</t>
+  </si>
+  <si>
+    <t>Verify that the number relevant individuals have been reduced to 3 from 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1. Open the online appointment form page.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2. Navigate to the relevant individual section.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>3. Add the relevant individuals and verify that only 3 individuals can be added at max.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>4. Verify that after adding three individuals, there is no link available for adding more individuals.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1. The new online appointment form page should be opened.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2. User scrolled down to the relevant individual section.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>3. Verified that only 3 individuals can be added at max.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>4. Link “Add more” is not displayed after adding three individuals</t>
+    </r>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>1.b</t>
+  </si>
+  <si>
+    <t>Verify that the company information questions have been reduce to 3 questions from 5.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1. Open the online appointment form page.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2. Scroll down to the company information questions.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">3. Verify that there are only 3 questions and they are: 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Is your company with 5 or more layers in its ownership / controlling structure?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Is your company directly or indirectly owned by a trust or foundation?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Does your company have any nominee shareholders in its ownership structure?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>1. The new online appointment form page should be opened.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>2. Scrolled down successfully.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>3. Verified that the question have ben reduced to 3 in numbers and are matching the expected questions from copywriting.</t>
+    </r>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
     <t>System Down Time</t>
   </si>
   <si>
-    <t>System healthy rate 81.67 %</t>
+    <t>System healthy rate 82.04 %</t>
   </si>
   <si>
     <t>Day</t>
@@ -6303,7 +6612,7 @@
     <t>Hours</t>
   </si>
   <si>
-    <t>out of 768 hours</t>
+    <t>out of 784 hours</t>
   </si>
   <si>
     <t>* Counting based on 8 working hours per day (1300-1400 lunch hour)</t>
@@ -7049,7 +7358,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -7657,6 +7966,9 @@
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -13940,7 +14252,7 @@
       </c>
       <c r="F4" s="142">
         <f>E4-NETWORKDAYS(TODAY(),D4,W1:W24)+1</f>
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="G4" s="143">
         <f>C24-E24</f>
@@ -13952,7 +14264,7 @@
       </c>
       <c r="I4" s="144">
         <f>IFERROR((F4/E4),0)</f>
-        <v>2.74285714285714</v>
+        <v>2.8</v>
       </c>
       <c r="J4" s="145">
         <f>H4/G4</f>
@@ -14103,15 +14415,15 @@
         <v>0</v>
       </c>
       <c r="C9" s="156">
-        <f>COUNTIFS('Test Cases'!$M1:$M110,"PA*",'Test Cases'!$L1:$L110,TODAY())</f>
+        <f>COUNTIFS('Test Cases'!$M1:$M143,"PA*",'Test Cases'!$L1:$L143,TODAY())</f>
         <v>0</v>
       </c>
       <c r="D9" s="157">
-        <f>COUNTIFS('Test Cases'!$M1:$M110,"Pe*",'Test Cases'!$L1:$L110,TODAY())</f>
+        <f>COUNTIFS('Test Cases'!$M1:$M143,"Pe*",'Test Cases'!$L1:$L143,TODAY())</f>
         <v>0</v>
       </c>
       <c r="E9" s="158">
-        <f>COUNTIFS('Test Cases'!$M1:$M110,"fA*",'Test Cases'!$L1:$L110,TODAY())</f>
+        <f>COUNTIFS('Test Cases'!$M1:$M143,"fA*",'Test Cases'!$L1:$L143,TODAY())</f>
         <v>0</v>
       </c>
       <c r="F9" s="137"/>
@@ -14263,7 +14575,7 @@
         <v>229</v>
       </c>
       <c r="C14" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Fulfillment*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Fulfillment*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="167">
@@ -14271,19 +14583,19 @@
         <v>0</v>
       </c>
       <c r="E14" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Fulfillment*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Fulfillment*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F14" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Fulfillment*",'Test Cases'!$M1:$M110,"Pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Fulfillment*",'Test Cases'!$M1:$M143,"Pa*")</f>
         <v>0</v>
       </c>
       <c r="G14" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Fulfillment*",'Test Cases'!$M1:$M110,"Pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Fulfillment*",'Test Cases'!$M1:$M143,"Pe*")</f>
         <v>0</v>
       </c>
       <c r="H14" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Fulfillment*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Fulfillment*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I14" s="170">
@@ -14320,7 +14632,7 @@
         <v>63</v>
       </c>
       <c r="C15" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Notifications*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Notifications*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="167">
@@ -14328,19 +14640,19 @@
         <v>0</v>
       </c>
       <c r="E15" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Notifications*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Notifications*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F15" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Notifications*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Notifications*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G15" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Notifications*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Notifications*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H15" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Notifications*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Notifications*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I15" s="170">
@@ -14377,7 +14689,7 @@
         <v>88</v>
       </c>
       <c r="C16" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Entry*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Entry*")</f>
         <v>0</v>
       </c>
       <c r="D16" s="167">
@@ -14385,19 +14697,19 @@
         <v>0</v>
       </c>
       <c r="E16" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Entry*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Entry*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F16" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Entry*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Entry*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G16" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Entry*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Entry*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H16" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Entry*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Entry*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I16" s="170">
@@ -14434,7 +14746,7 @@
         <v>102</v>
       </c>
       <c r="C17" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Statements*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Statements*")</f>
         <v>0</v>
       </c>
       <c r="D17" s="167">
@@ -14442,19 +14754,19 @@
         <v>0</v>
       </c>
       <c r="E17" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Statements*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Statements*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F17" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Statements*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Statements*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G17" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Statements*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Statements*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H17" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Statements*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Statements*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I17" s="170">
@@ -14491,7 +14803,7 @@
         <v>107</v>
       </c>
       <c r="C18" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Referee*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Referee*")</f>
         <v>0</v>
       </c>
       <c r="D18" s="167">
@@ -14499,19 +14811,19 @@
         <v>0</v>
       </c>
       <c r="E18" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referee*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referee*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F18" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referee*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referee*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G18" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referee*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referee*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H18" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referee*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referee*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I18" s="170">
@@ -14548,7 +14860,7 @@
         <v>116</v>
       </c>
       <c r="C19" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"BO*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"BO*")</f>
         <v>0</v>
       </c>
       <c r="D19" s="167">
@@ -14556,19 +14868,19 @@
         <v>0</v>
       </c>
       <c r="E19" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"BO*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"BO*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F19" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"BO*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"BO*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G19" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"BO*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"BO*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H19" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"BO*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"BO*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I19" s="170">
@@ -14605,7 +14917,7 @@
         <v>230</v>
       </c>
       <c r="C20" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Referrer*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Referrer*")</f>
         <v>0</v>
       </c>
       <c r="D20" s="167">
@@ -14613,19 +14925,19 @@
         <v>0</v>
       </c>
       <c r="E20" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referrer*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referrer*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F20" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referrer*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referrer*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G20" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referrer*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referrer*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H20" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Referrer*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Referrer*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I20" s="170">
@@ -14662,7 +14974,7 @@
         <v>29</v>
       </c>
       <c r="C21" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Reports*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Reports*")</f>
         <v>0</v>
       </c>
       <c r="D21" s="167">
@@ -14670,19 +14982,19 @@
         <v>0</v>
       </c>
       <c r="E21" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Reports*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Reports*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F21" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Reports*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Reports*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G21" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Reports*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Reports*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H21" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Reports*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Reports*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I21" s="170">
@@ -14719,7 +15031,7 @@
         <v>182</v>
       </c>
       <c r="C22" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Data*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Data*")</f>
         <v>0</v>
       </c>
       <c r="D22" s="167">
@@ -14727,19 +15039,19 @@
         <v>0</v>
       </c>
       <c r="E22" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Data*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Data*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F22" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Data*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Data*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G22" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Data*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Data*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H22" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Data*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Data*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I22" s="170">
@@ -14776,7 +15088,7 @@
         <v>189</v>
       </c>
       <c r="C23" s="155">
-        <f>COUNTIF('Test Cases'!$B1:$B110,"Others*")</f>
+        <f>COUNTIF('Test Cases'!$B1:$B143,"Others*")</f>
         <v>0</v>
       </c>
       <c r="D23" s="167">
@@ -14784,19 +15096,19 @@
         <v>0</v>
       </c>
       <c r="E23" s="168">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Others*",'Test Cases'!$M1:$M110,"Can*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Others*",'Test Cases'!$M1:$M143,"Can*")</f>
         <v>0</v>
       </c>
       <c r="F23" s="156">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Others*",'Test Cases'!$M1:$M110,"pa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Others*",'Test Cases'!$M1:$M143,"pa*")</f>
         <v>0</v>
       </c>
       <c r="G23" s="157">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Others*",'Test Cases'!$M1:$M110,"pe*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Others*",'Test Cases'!$M1:$M143,"pe*")</f>
         <v>0</v>
       </c>
       <c r="H23" s="169">
-        <f>COUNTIFS('Test Cases'!$B1:$B110,"Others*",'Test Cases'!$M1:$M110,"fa*")</f>
+        <f>COUNTIFS('Test Cases'!$B1:$B143,"Others*",'Test Cases'!$M1:$M143,"fa*")</f>
         <v>0</v>
       </c>
       <c r="I23" s="170">
@@ -14895,7 +15207,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N110"/>
+  <dimension ref="A1:N143"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -18863,6 +19175,854 @@
       </c>
       <c r="N110" s="198"/>
     </row>
+    <row r="111" ht="28" customHeight="1">
+      <c r="A111" t="s" s="193">
+        <v>425</v>
+      </c>
+      <c r="B111" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C111" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D111" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E111" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F111" t="s" s="193">
+        <v>247</v>
+      </c>
+      <c r="G111" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H111" s="196"/>
+      <c r="I111" s="196"/>
+      <c r="J111" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K111" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L111" s="197"/>
+      <c r="M111" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N111" s="198"/>
+    </row>
+    <row r="112" ht="28" customHeight="1">
+      <c r="A112" t="s" s="193">
+        <v>431</v>
+      </c>
+      <c r="B112" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C112" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D112" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E112" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F112" t="s" s="193">
+        <v>247</v>
+      </c>
+      <c r="G112" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H112" s="196"/>
+      <c r="I112" s="196"/>
+      <c r="J112" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K112" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L112" s="197"/>
+      <c r="M112" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N112" s="198"/>
+    </row>
+    <row r="113" ht="28" customHeight="1">
+      <c r="A113" t="s" s="193">
+        <v>436</v>
+      </c>
+      <c r="B113" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C113" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D113" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E113" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F113" t="s" s="193">
+        <v>352</v>
+      </c>
+      <c r="G113" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H113" s="196"/>
+      <c r="I113" s="196"/>
+      <c r="J113" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K113" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L113" s="197"/>
+      <c r="M113" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N113" s="198"/>
+    </row>
+    <row r="114" ht="28" customHeight="1">
+      <c r="A114" t="s" s="193">
+        <v>437</v>
+      </c>
+      <c r="B114" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C114" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D114" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E114" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F114" t="s" s="193">
+        <v>352</v>
+      </c>
+      <c r="G114" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H114" s="196"/>
+      <c r="I114" s="196"/>
+      <c r="J114" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K114" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L114" s="197"/>
+      <c r="M114" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N114" s="198"/>
+    </row>
+    <row r="115" ht="28" customHeight="1">
+      <c r="A115" t="s" s="193">
+        <v>438</v>
+      </c>
+      <c r="B115" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C115" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D115" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E115" t="s" s="193">
+        <v>324</v>
+      </c>
+      <c r="F115" t="s" s="193">
+        <v>247</v>
+      </c>
+      <c r="G115" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H115" s="196"/>
+      <c r="I115" s="196"/>
+      <c r="J115" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K115" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L115" s="197"/>
+      <c r="M115" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N115" s="198"/>
+    </row>
+    <row r="116" ht="28" customHeight="1">
+      <c r="A116" t="s" s="193">
+        <v>439</v>
+      </c>
+      <c r="B116" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C116" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D116" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E116" t="s" s="193">
+        <v>324</v>
+      </c>
+      <c r="F116" t="s" s="193">
+        <v>247</v>
+      </c>
+      <c r="G116" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H116" s="196"/>
+      <c r="I116" s="196"/>
+      <c r="J116" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K116" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L116" s="197"/>
+      <c r="M116" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N116" s="198"/>
+    </row>
+    <row r="117" ht="28" customHeight="1">
+      <c r="A117" t="s" s="193">
+        <v>440</v>
+      </c>
+      <c r="B117" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C117" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D117" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E117" t="s" s="193">
+        <v>324</v>
+      </c>
+      <c r="F117" t="s" s="193">
+        <v>352</v>
+      </c>
+      <c r="G117" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H117" s="196"/>
+      <c r="I117" s="196"/>
+      <c r="J117" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K117" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L117" s="197"/>
+      <c r="M117" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N117" s="198"/>
+    </row>
+    <row r="118" ht="28" customHeight="1">
+      <c r="A118" t="s" s="193">
+        <v>441</v>
+      </c>
+      <c r="B118" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C118" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D118" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E118" t="s" s="193">
+        <v>324</v>
+      </c>
+      <c r="F118" t="s" s="193">
+        <v>352</v>
+      </c>
+      <c r="G118" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H118" s="196"/>
+      <c r="I118" s="196"/>
+      <c r="J118" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K118" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L118" s="197"/>
+      <c r="M118" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N118" s="198"/>
+    </row>
+    <row r="119" ht="28" customHeight="1">
+      <c r="A119" t="s" s="193">
+        <v>442</v>
+      </c>
+      <c r="B119" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C119" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D119" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E119" t="s" s="193">
+        <v>338</v>
+      </c>
+      <c r="F119" t="s" s="193">
+        <v>247</v>
+      </c>
+      <c r="G119" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H119" s="196"/>
+      <c r="I119" s="196"/>
+      <c r="J119" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K119" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L119" s="197"/>
+      <c r="M119" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N119" s="198"/>
+    </row>
+    <row r="120" ht="28" customHeight="1">
+      <c r="A120" t="s" s="193">
+        <v>443</v>
+      </c>
+      <c r="B120" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C120" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D120" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E120" t="s" s="193">
+        <v>338</v>
+      </c>
+      <c r="F120" t="s" s="193">
+        <v>247</v>
+      </c>
+      <c r="G120" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H120" s="196"/>
+      <c r="I120" s="196"/>
+      <c r="J120" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K120" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L120" s="197"/>
+      <c r="M120" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N120" s="198"/>
+    </row>
+    <row r="121" ht="28" customHeight="1">
+      <c r="A121" t="s" s="193">
+        <v>444</v>
+      </c>
+      <c r="B121" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C121" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D121" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E121" t="s" s="193">
+        <v>338</v>
+      </c>
+      <c r="F121" t="s" s="193">
+        <v>352</v>
+      </c>
+      <c r="G121" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H121" s="196"/>
+      <c r="I121" s="196"/>
+      <c r="J121" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K121" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L121" s="197"/>
+      <c r="M121" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N121" s="198"/>
+    </row>
+    <row r="122" ht="28" customHeight="1">
+      <c r="A122" t="s" s="193">
+        <v>445</v>
+      </c>
+      <c r="B122" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C122" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D122" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E122" t="s" s="193">
+        <v>338</v>
+      </c>
+      <c r="F122" t="s" s="193">
+        <v>352</v>
+      </c>
+      <c r="G122" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H122" s="196"/>
+      <c r="I122" s="196"/>
+      <c r="J122" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K122" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L122" s="197"/>
+      <c r="M122" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N122" s="198"/>
+    </row>
+    <row r="123" ht="28" customHeight="1">
+      <c r="A123" t="s" s="193">
+        <v>446</v>
+      </c>
+      <c r="B123" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C123" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D123" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E123" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F123" t="s" s="193">
+        <v>411</v>
+      </c>
+      <c r="G123" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H123" s="196"/>
+      <c r="I123" s="196"/>
+      <c r="J123" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K123" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L123" s="197"/>
+      <c r="M123" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N123" s="198"/>
+    </row>
+    <row r="124" ht="28" customHeight="1">
+      <c r="A124" t="s" s="193">
+        <v>447</v>
+      </c>
+      <c r="B124" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C124" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D124" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E124" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F124" t="s" s="193">
+        <v>411</v>
+      </c>
+      <c r="G124" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H124" s="196"/>
+      <c r="I124" s="196"/>
+      <c r="J124" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K124" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L124" s="197"/>
+      <c r="M124" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N124" s="198"/>
+    </row>
+    <row r="125" ht="28" customHeight="1">
+      <c r="A125" t="s" s="193">
+        <v>448</v>
+      </c>
+      <c r="B125" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C125" t="s" s="193">
+        <v>427</v>
+      </c>
+      <c r="D125" t="s" s="200">
+        <v>428</v>
+      </c>
+      <c r="E125" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F125" t="s" s="193">
+        <v>393</v>
+      </c>
+      <c r="G125" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H125" s="196"/>
+      <c r="I125" s="196"/>
+      <c r="J125" t="s" s="195">
+        <v>429</v>
+      </c>
+      <c r="K125" t="s" s="195">
+        <v>430</v>
+      </c>
+      <c r="L125" s="197"/>
+      <c r="M125" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N125" s="198"/>
+    </row>
+    <row r="126" ht="28" customHeight="1">
+      <c r="A126" t="s" s="193">
+        <v>449</v>
+      </c>
+      <c r="B126" t="s" s="193">
+        <v>426</v>
+      </c>
+      <c r="C126" t="s" s="193">
+        <v>432</v>
+      </c>
+      <c r="D126" t="s" s="200">
+        <v>433</v>
+      </c>
+      <c r="E126" t="s" s="193">
+        <v>246</v>
+      </c>
+      <c r="F126" t="s" s="193">
+        <v>393</v>
+      </c>
+      <c r="G126" t="s" s="195">
+        <v>272</v>
+      </c>
+      <c r="H126" s="196"/>
+      <c r="I126" s="196"/>
+      <c r="J126" t="s" s="195">
+        <v>434</v>
+      </c>
+      <c r="K126" t="s" s="195">
+        <v>435</v>
+      </c>
+      <c r="L126" s="197"/>
+      <c r="M126" t="s" s="193">
+        <v>251</v>
+      </c>
+      <c r="N126" s="198"/>
+    </row>
+    <row r="127" ht="28" customHeight="1">
+      <c r="A127" s="198"/>
+      <c r="B127" s="198"/>
+      <c r="C127" s="198"/>
+      <c r="D127" s="203"/>
+      <c r="E127" s="198"/>
+      <c r="F127" s="198"/>
+      <c r="G127" s="196"/>
+      <c r="H127" s="196"/>
+      <c r="I127" s="196"/>
+      <c r="J127" s="196"/>
+      <c r="K127" s="196"/>
+      <c r="L127" s="197"/>
+      <c r="M127" s="198"/>
+      <c r="N127" s="198"/>
+    </row>
+    <row r="128" ht="28" customHeight="1">
+      <c r="A128" s="198"/>
+      <c r="B128" s="198"/>
+      <c r="C128" s="198"/>
+      <c r="D128" s="203"/>
+      <c r="E128" s="198"/>
+      <c r="F128" s="198"/>
+      <c r="G128" s="196"/>
+      <c r="H128" s="196"/>
+      <c r="I128" s="196"/>
+      <c r="J128" s="196"/>
+      <c r="K128" s="196"/>
+      <c r="L128" s="197"/>
+      <c r="M128" s="198"/>
+      <c r="N128" s="198"/>
+    </row>
+    <row r="129" ht="28" customHeight="1">
+      <c r="A129" s="198"/>
+      <c r="B129" s="198"/>
+      <c r="C129" s="198"/>
+      <c r="D129" s="203"/>
+      <c r="E129" s="198"/>
+      <c r="F129" s="198"/>
+      <c r="G129" s="196"/>
+      <c r="H129" s="196"/>
+      <c r="I129" s="196"/>
+      <c r="J129" s="196"/>
+      <c r="K129" s="196"/>
+      <c r="L129" s="197"/>
+      <c r="M129" s="198"/>
+      <c r="N129" s="198"/>
+    </row>
+    <row r="130" ht="28" customHeight="1">
+      <c r="A130" s="198"/>
+      <c r="B130" s="198"/>
+      <c r="C130" s="198"/>
+      <c r="D130" s="203"/>
+      <c r="E130" s="198"/>
+      <c r="F130" s="198"/>
+      <c r="G130" s="196"/>
+      <c r="H130" s="196"/>
+      <c r="I130" s="196"/>
+      <c r="J130" s="196"/>
+      <c r="K130" s="196"/>
+      <c r="L130" s="197"/>
+      <c r="M130" s="198"/>
+      <c r="N130" s="198"/>
+    </row>
+    <row r="131" ht="28" customHeight="1">
+      <c r="A131" s="198"/>
+      <c r="B131" s="198"/>
+      <c r="C131" s="198"/>
+      <c r="D131" s="203"/>
+      <c r="E131" s="198"/>
+      <c r="F131" s="198"/>
+      <c r="G131" s="196"/>
+      <c r="H131" s="196"/>
+      <c r="I131" s="196"/>
+      <c r="J131" s="196"/>
+      <c r="K131" s="196"/>
+      <c r="L131" s="197"/>
+      <c r="M131" s="198"/>
+      <c r="N131" s="198"/>
+    </row>
+    <row r="132" ht="28" customHeight="1">
+      <c r="A132" s="198"/>
+      <c r="B132" s="198"/>
+      <c r="C132" s="198"/>
+      <c r="D132" s="203"/>
+      <c r="E132" s="198"/>
+      <c r="F132" s="198"/>
+      <c r="G132" s="196"/>
+      <c r="H132" s="196"/>
+      <c r="I132" s="196"/>
+      <c r="J132" s="196"/>
+      <c r="K132" s="196"/>
+      <c r="L132" s="197"/>
+      <c r="M132" s="198"/>
+      <c r="N132" s="198"/>
+    </row>
+    <row r="133" ht="28" customHeight="1">
+      <c r="A133" s="198"/>
+      <c r="B133" s="198"/>
+      <c r="C133" s="198"/>
+      <c r="D133" s="203"/>
+      <c r="E133" s="198"/>
+      <c r="F133" s="198"/>
+      <c r="G133" s="196"/>
+      <c r="H133" s="196"/>
+      <c r="I133" s="196"/>
+      <c r="J133" s="196"/>
+      <c r="K133" s="196"/>
+      <c r="L133" s="197"/>
+      <c r="M133" s="198"/>
+      <c r="N133" s="198"/>
+    </row>
+    <row r="134" ht="28" customHeight="1">
+      <c r="A134" s="198"/>
+      <c r="B134" s="198"/>
+      <c r="C134" s="198"/>
+      <c r="D134" s="203"/>
+      <c r="E134" s="198"/>
+      <c r="F134" s="198"/>
+      <c r="G134" s="196"/>
+      <c r="H134" s="196"/>
+      <c r="I134" s="196"/>
+      <c r="J134" s="196"/>
+      <c r="K134" s="196"/>
+      <c r="L134" s="197"/>
+      <c r="M134" s="198"/>
+      <c r="N134" s="198"/>
+    </row>
+    <row r="135" ht="28" customHeight="1">
+      <c r="A135" s="198"/>
+      <c r="B135" s="198"/>
+      <c r="C135" s="198"/>
+      <c r="D135" s="203"/>
+      <c r="E135" s="198"/>
+      <c r="F135" s="198"/>
+      <c r="G135" s="196"/>
+      <c r="H135" s="196"/>
+      <c r="I135" s="196"/>
+      <c r="J135" s="196"/>
+      <c r="K135" s="196"/>
+      <c r="L135" s="197"/>
+      <c r="M135" s="198"/>
+      <c r="N135" s="198"/>
+    </row>
+    <row r="136" ht="28" customHeight="1">
+      <c r="A136" s="198"/>
+      <c r="B136" s="198"/>
+      <c r="C136" s="198"/>
+      <c r="D136" s="203"/>
+      <c r="E136" s="198"/>
+      <c r="F136" s="198"/>
+      <c r="G136" s="196"/>
+      <c r="H136" s="196"/>
+      <c r="I136" s="196"/>
+      <c r="J136" s="196"/>
+      <c r="K136" s="196"/>
+      <c r="L136" s="197"/>
+      <c r="M136" s="198"/>
+      <c r="N136" s="198"/>
+    </row>
+    <row r="137" ht="28" customHeight="1">
+      <c r="A137" s="198"/>
+      <c r="B137" s="198"/>
+      <c r="C137" s="198"/>
+      <c r="D137" s="203"/>
+      <c r="E137" s="198"/>
+      <c r="F137" s="198"/>
+      <c r="G137" s="196"/>
+      <c r="H137" s="196"/>
+      <c r="I137" s="196"/>
+      <c r="J137" s="196"/>
+      <c r="K137" s="196"/>
+      <c r="L137" s="197"/>
+      <c r="M137" s="198"/>
+      <c r="N137" s="198"/>
+    </row>
+    <row r="138" ht="28" customHeight="1">
+      <c r="A138" s="198"/>
+      <c r="B138" s="198"/>
+      <c r="C138" s="198"/>
+      <c r="D138" s="203"/>
+      <c r="E138" s="198"/>
+      <c r="F138" s="198"/>
+      <c r="G138" s="196"/>
+      <c r="H138" s="196"/>
+      <c r="I138" s="196"/>
+      <c r="J138" s="196"/>
+      <c r="K138" s="196"/>
+      <c r="L138" s="197"/>
+      <c r="M138" s="198"/>
+      <c r="N138" s="198"/>
+    </row>
+    <row r="139" ht="28" customHeight="1">
+      <c r="A139" s="198"/>
+      <c r="B139" s="198"/>
+      <c r="C139" s="198"/>
+      <c r="D139" s="203"/>
+      <c r="E139" s="198"/>
+      <c r="F139" s="198"/>
+      <c r="G139" s="196"/>
+      <c r="H139" s="196"/>
+      <c r="I139" s="196"/>
+      <c r="J139" s="196"/>
+      <c r="K139" s="196"/>
+      <c r="L139" s="197"/>
+      <c r="M139" s="198"/>
+      <c r="N139" s="198"/>
+    </row>
+    <row r="140" ht="28" customHeight="1">
+      <c r="A140" s="198"/>
+      <c r="B140" s="198"/>
+      <c r="C140" s="198"/>
+      <c r="D140" s="203"/>
+      <c r="E140" s="198"/>
+      <c r="F140" s="198"/>
+      <c r="G140" s="196"/>
+      <c r="H140" s="196"/>
+      <c r="I140" s="196"/>
+      <c r="J140" s="196"/>
+      <c r="K140" s="196"/>
+      <c r="L140" s="197"/>
+      <c r="M140" s="198"/>
+      <c r="N140" s="198"/>
+    </row>
+    <row r="141" ht="28" customHeight="1">
+      <c r="A141" s="198"/>
+      <c r="B141" s="198"/>
+      <c r="C141" s="198"/>
+      <c r="D141" s="203"/>
+      <c r="E141" s="198"/>
+      <c r="F141" s="198"/>
+      <c r="G141" s="196"/>
+      <c r="H141" s="196"/>
+      <c r="I141" s="196"/>
+      <c r="J141" s="196"/>
+      <c r="K141" s="196"/>
+      <c r="L141" s="197"/>
+      <c r="M141" s="198"/>
+      <c r="N141" s="198"/>
+    </row>
+    <row r="142" ht="28" customHeight="1">
+      <c r="A142" s="198"/>
+      <c r="B142" s="198"/>
+      <c r="C142" s="198"/>
+      <c r="D142" s="203"/>
+      <c r="E142" s="198"/>
+      <c r="F142" s="198"/>
+      <c r="G142" s="196"/>
+      <c r="H142" s="196"/>
+      <c r="I142" s="196"/>
+      <c r="J142" s="196"/>
+      <c r="K142" s="196"/>
+      <c r="L142" s="197"/>
+      <c r="M142" s="198"/>
+      <c r="N142" s="198"/>
+    </row>
+    <row r="143" ht="28" customHeight="1">
+      <c r="A143" s="198"/>
+      <c r="B143" s="198"/>
+      <c r="C143" s="198"/>
+      <c r="D143" s="203"/>
+      <c r="E143" s="198"/>
+      <c r="F143" s="198"/>
+      <c r="G143" s="196"/>
+      <c r="H143" s="196"/>
+      <c r="I143" s="196"/>
+      <c r="J143" s="196"/>
+      <c r="K143" s="196"/>
+      <c r="L143" s="197"/>
+      <c r="M143" s="198"/>
+      <c r="N143" s="198"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -18880,15 +20040,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="14.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="8.85156" style="203" customWidth="1"/>
-    <col min="2" max="2" width="20.3516" style="203" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="203" customWidth="1"/>
-    <col min="4" max="4" width="14.3516" style="203" customWidth="1"/>
-    <col min="5" max="5" width="15.3516" style="203" customWidth="1"/>
-    <col min="6" max="6" width="43.8516" style="203" customWidth="1"/>
-    <col min="7" max="7" width="23.5" style="203" customWidth="1"/>
-    <col min="8" max="8" width="48.6719" style="203" customWidth="1"/>
-    <col min="9" max="256" width="8.85156" style="203" customWidth="1"/>
+    <col min="1" max="1" width="8.85156" style="204" customWidth="1"/>
+    <col min="2" max="2" width="20.3516" style="204" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="204" customWidth="1"/>
+    <col min="4" max="4" width="14.3516" style="204" customWidth="1"/>
+    <col min="5" max="5" width="15.3516" style="204" customWidth="1"/>
+    <col min="6" max="6" width="43.8516" style="204" customWidth="1"/>
+    <col min="7" max="7" width="23.5" style="204" customWidth="1"/>
+    <col min="8" max="8" width="48.6719" style="204" customWidth="1"/>
+    <col min="9" max="256" width="8.85156" style="204" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16" customHeight="1">
@@ -18903,857 +20063,857 @@
     </row>
     <row r="2" ht="16" customHeight="1">
       <c r="A2" s="123"/>
-      <c r="B2" t="s" s="204">
-        <v>425</v>
+      <c r="B2" t="s" s="205">
+        <v>450</v>
       </c>
       <c r="C2" s="126"/>
-      <c r="D2" s="205"/>
-      <c r="E2" s="205"/>
-      <c r="F2" s="205"/>
-      <c r="G2" s="205"/>
-      <c r="H2" s="206"/>
+      <c r="D2" s="206"/>
+      <c r="E2" s="206"/>
+      <c r="F2" s="206"/>
+      <c r="G2" s="206"/>
+      <c r="H2" s="207"/>
     </row>
     <row r="3" ht="16" customHeight="1">
       <c r="A3" s="123"/>
-      <c r="B3" s="207"/>
+      <c r="B3" s="208"/>
       <c r="C3" s="126"/>
-      <c r="D3" s="205"/>
-      <c r="E3" s="205"/>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="206"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="206"/>
+      <c r="G3" s="206"/>
+      <c r="H3" s="207"/>
     </row>
     <row r="4" ht="16" customHeight="1">
       <c r="A4" s="123"/>
-      <c r="B4" t="s" s="208">
+      <c r="B4" t="s" s="209">
         <f>"System healthy rate "&amp;(1-ROUNDUP(E41/(8*('UAT Status'!E4-NETWORKDAYS(TODAY(),'UAT Status'!D4,'UAT Status'!W1:W24)+1)),4))*100&amp;" %"</f>
-        <v>426</v>
-      </c>
-      <c r="C4" s="209"/>
-      <c r="D4" s="209"/>
-      <c r="E4" s="209"/>
-      <c r="F4" s="209"/>
-      <c r="G4" s="209"/>
-      <c r="H4" s="210"/>
+        <v>451</v>
+      </c>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
+      <c r="E4" s="210"/>
+      <c r="F4" s="210"/>
+      <c r="G4" s="210"/>
+      <c r="H4" s="211"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="211"/>
+      <c r="A5" s="212"/>
       <c r="B5" t="s" s="5">
-        <v>427</v>
+        <v>452</v>
       </c>
       <c r="C5" t="s" s="5">
-        <v>428</v>
+        <v>453</v>
       </c>
       <c r="D5" t="s" s="5">
-        <v>429</v>
+        <v>454</v>
       </c>
       <c r="E5" t="s" s="5">
-        <v>430</v>
+        <v>455</v>
       </c>
       <c r="F5" t="s" s="5">
-        <v>431</v>
+        <v>456</v>
       </c>
       <c r="G5" t="s" s="5">
-        <v>432</v>
+        <v>457</v>
       </c>
       <c r="H5" t="s" s="5">
-        <v>433</v>
+        <v>458</v>
       </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="211"/>
-      <c r="B6" s="212">
+      <c r="A6" s="212"/>
+      <c r="B6" s="213">
         <v>1</v>
       </c>
-      <c r="C6" s="213">
+      <c r="C6" s="214">
         <v>44095</v>
       </c>
-      <c r="D6" t="s" s="214">
-        <v>434</v>
-      </c>
-      <c r="E6" s="212">
+      <c r="D6" t="s" s="215">
+        <v>459</v>
+      </c>
+      <c r="E6" s="213">
         <v>8</v>
       </c>
       <c r="F6" t="s" s="193">
-        <v>435</v>
+        <v>460</v>
       </c>
       <c r="G6" t="s" s="195">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H6" t="s" s="195">
-        <v>437</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="211"/>
-      <c r="B7" s="212">
+      <c r="A7" s="212"/>
+      <c r="B7" s="213">
         <v>2</v>
       </c>
-      <c r="C7" s="213">
+      <c r="C7" s="214">
         <v>44096</v>
       </c>
-      <c r="D7" t="s" s="214">
-        <v>434</v>
-      </c>
-      <c r="E7" s="212">
+      <c r="D7" t="s" s="215">
+        <v>459</v>
+      </c>
+      <c r="E7" s="213">
         <v>8</v>
       </c>
       <c r="F7" t="s" s="193">
-        <v>435</v>
+        <v>460</v>
       </c>
       <c r="G7" t="s" s="195">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H7" t="s" s="195">
-        <v>437</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="211"/>
-      <c r="B8" s="212">
+      <c r="A8" s="212"/>
+      <c r="B8" s="213">
         <v>3</v>
       </c>
-      <c r="C8" s="213">
+      <c r="C8" s="214">
         <v>44097</v>
       </c>
-      <c r="D8" t="s" s="214">
-        <v>438</v>
-      </c>
-      <c r="E8" s="212">
+      <c r="D8" t="s" s="215">
+        <v>463</v>
+      </c>
+      <c r="E8" s="213">
         <v>2.5</v>
       </c>
       <c r="F8" t="s" s="193">
-        <v>439</v>
+        <v>464</v>
       </c>
       <c r="G8" t="s" s="195">
-        <v>436</v>
-      </c>
-      <c r="H8" t="s" s="215">
-        <v>440</v>
+        <v>461</v>
+      </c>
+      <c r="H8" t="s" s="216">
+        <v>465</v>
       </c>
     </row>
     <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="211"/>
-      <c r="B9" s="212">
+      <c r="A9" s="212"/>
+      <c r="B9" s="213">
         <v>4</v>
       </c>
-      <c r="C9" s="213">
+      <c r="C9" s="214">
         <v>44098</v>
       </c>
-      <c r="D9" t="s" s="214">
-        <v>441</v>
-      </c>
-      <c r="E9" s="212">
+      <c r="D9" t="s" s="215">
+        <v>466</v>
+      </c>
+      <c r="E9" s="213">
         <v>1.75</v>
       </c>
       <c r="F9" t="s" s="193">
-        <v>442</v>
+        <v>467</v>
       </c>
       <c r="G9" t="s" s="195">
-        <v>436</v>
-      </c>
-      <c r="H9" t="s" s="215">
-        <v>443</v>
+        <v>461</v>
+      </c>
+      <c r="H9" t="s" s="216">
+        <v>468</v>
       </c>
     </row>
     <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="211"/>
-      <c r="B10" s="212">
+      <c r="A10" s="212"/>
+      <c r="B10" s="213">
         <v>5</v>
       </c>
-      <c r="C10" s="213">
+      <c r="C10" s="214">
         <v>44099</v>
       </c>
-      <c r="D10" t="s" s="214">
-        <v>444</v>
-      </c>
-      <c r="E10" s="212">
+      <c r="D10" t="s" s="215">
+        <v>469</v>
+      </c>
+      <c r="E10" s="213">
         <v>5</v>
       </c>
       <c r="F10" t="s" s="193">
-        <v>442</v>
+        <v>467</v>
       </c>
       <c r="G10" t="s" s="195">
-        <v>436</v>
-      </c>
-      <c r="H10" t="s" s="215">
-        <v>445</v>
+        <v>461</v>
+      </c>
+      <c r="H10" t="s" s="216">
+        <v>470</v>
       </c>
     </row>
     <row r="11" ht="28.5" customHeight="1">
-      <c r="A11" s="211"/>
-      <c r="B11" s="212">
+      <c r="A11" s="212"/>
+      <c r="B11" s="213">
         <v>6</v>
       </c>
-      <c r="C11" s="213">
+      <c r="C11" s="214">
         <v>44102</v>
       </c>
-      <c r="D11" t="s" s="216">
-        <v>446</v>
-      </c>
-      <c r="E11" s="212">
+      <c r="D11" t="s" s="217">
+        <v>471</v>
+      </c>
+      <c r="E11" s="213">
         <v>8</v>
       </c>
       <c r="F11" t="s" s="195">
-        <v>447</v>
-      </c>
-      <c r="G11" t="s" s="217">
-        <v>448</v>
-      </c>
-      <c r="H11" t="s" s="217">
-        <v>449</v>
+        <v>472</v>
+      </c>
+      <c r="G11" t="s" s="218">
+        <v>473</v>
+      </c>
+      <c r="H11" t="s" s="218">
+        <v>474</v>
       </c>
     </row>
     <row r="12" ht="28.5" customHeight="1">
-      <c r="A12" s="211"/>
-      <c r="B12" s="212">
+      <c r="A12" s="212"/>
+      <c r="B12" s="213">
         <v>7</v>
       </c>
-      <c r="C12" s="213">
+      <c r="C12" s="214">
         <v>44103</v>
       </c>
-      <c r="D12" t="s" s="216">
-        <v>450</v>
-      </c>
-      <c r="E12" s="212">
+      <c r="D12" t="s" s="217">
+        <v>475</v>
+      </c>
+      <c r="E12" s="213">
         <v>5</v>
       </c>
       <c r="F12" t="s" s="195">
-        <v>451</v>
-      </c>
-      <c r="G12" t="s" s="217">
-        <v>452</v>
+        <v>476</v>
+      </c>
+      <c r="G12" t="s" s="218">
+        <v>477</v>
       </c>
       <c r="H12" t="s" s="195">
-        <v>453</v>
+        <v>478</v>
       </c>
     </row>
     <row r="13" ht="28.5" customHeight="1">
-      <c r="A13" s="211"/>
-      <c r="B13" s="212">
+      <c r="A13" s="212"/>
+      <c r="B13" s="213">
         <v>8</v>
       </c>
-      <c r="C13" s="213">
+      <c r="C13" s="214">
         <v>44104</v>
       </c>
-      <c r="D13" t="s" s="216">
-        <v>454</v>
-      </c>
-      <c r="E13" s="212">
+      <c r="D13" t="s" s="217">
+        <v>479</v>
+      </c>
+      <c r="E13" s="213">
         <v>4.5</v>
       </c>
       <c r="F13" t="s" s="195">
-        <v>455</v>
-      </c>
-      <c r="G13" t="s" s="217">
-        <v>456</v>
+        <v>480</v>
+      </c>
+      <c r="G13" t="s" s="218">
+        <v>481</v>
       </c>
       <c r="H13" t="s" s="195">
-        <v>453</v>
+        <v>478</v>
       </c>
     </row>
     <row r="14" ht="16" customHeight="1">
-      <c r="A14" s="211"/>
-      <c r="B14" s="212">
+      <c r="A14" s="212"/>
+      <c r="B14" s="213">
         <v>9</v>
       </c>
-      <c r="C14" s="213">
+      <c r="C14" s="214">
         <v>44109</v>
       </c>
-      <c r="D14" t="s" s="214">
-        <v>434</v>
-      </c>
-      <c r="E14" s="212">
+      <c r="D14" t="s" s="215">
+        <v>459</v>
+      </c>
+      <c r="E14" s="213">
         <v>8</v>
       </c>
       <c r="F14" t="s" s="193">
-        <v>457</v>
+        <v>482</v>
       </c>
       <c r="G14" t="s" s="195">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H14" t="s" s="195">
-        <v>458</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15" ht="16" customHeight="1">
-      <c r="A15" s="211"/>
-      <c r="B15" s="212">
+      <c r="A15" s="212"/>
+      <c r="B15" s="213">
         <v>10</v>
       </c>
-      <c r="C15" s="213">
+      <c r="C15" s="214">
         <v>44110</v>
       </c>
-      <c r="D15" t="s" s="214">
-        <v>459</v>
-      </c>
-      <c r="E15" s="212">
+      <c r="D15" t="s" s="215">
+        <v>484</v>
+      </c>
+      <c r="E15" s="213">
         <v>7</v>
       </c>
       <c r="F15" t="s" s="193">
-        <v>457</v>
+        <v>482</v>
       </c>
       <c r="G15" t="s" s="195">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H15" t="s" s="195">
-        <v>460</v>
+        <v>485</v>
       </c>
     </row>
     <row r="16" ht="16" customHeight="1">
-      <c r="A16" s="211"/>
-      <c r="B16" s="212">
+      <c r="A16" s="212"/>
+      <c r="B16" s="213">
         <v>11</v>
       </c>
-      <c r="C16" s="213">
+      <c r="C16" s="214">
         <v>44111</v>
       </c>
-      <c r="D16" t="s" s="214">
-        <v>459</v>
-      </c>
-      <c r="E16" s="212">
+      <c r="D16" t="s" s="215">
+        <v>484</v>
+      </c>
+      <c r="E16" s="213">
         <v>7</v>
       </c>
       <c r="F16" t="s" s="193">
+        <v>486</v>
+      </c>
+      <c r="G16" t="s" s="216">
+        <v>487</v>
+      </c>
+      <c r="H16" t="s" s="216">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="17" ht="42" customHeight="1">
+      <c r="A17" s="212"/>
+      <c r="B17" s="213">
+        <v>12</v>
+      </c>
+      <c r="C17" s="214">
+        <v>44112</v>
+      </c>
+      <c r="D17" t="s" s="217">
+        <v>489</v>
+      </c>
+      <c r="E17" s="213">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s" s="195">
+        <v>490</v>
+      </c>
+      <c r="G17" t="s" s="195">
+        <v>491</v>
+      </c>
+      <c r="H17" t="s" s="195">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="18" ht="16" customHeight="1">
+      <c r="A18" s="212"/>
+      <c r="B18" s="213">
+        <v>13</v>
+      </c>
+      <c r="C18" s="214">
+        <v>44113</v>
+      </c>
+      <c r="D18" t="s" s="215">
+        <v>463</v>
+      </c>
+      <c r="E18" s="213">
+        <v>2.5</v>
+      </c>
+      <c r="F18" t="s" s="193">
+        <v>493</v>
+      </c>
+      <c r="G18" t="s" s="193">
         <v>461</v>
       </c>
-      <c r="G16" t="s" s="215">
-        <v>462</v>
-      </c>
-      <c r="H16" t="s" s="215">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="17" ht="42" customHeight="1">
-      <c r="A17" s="211"/>
-      <c r="B17" s="212">
-        <v>12</v>
-      </c>
-      <c r="C17" s="213">
-        <v>44112</v>
-      </c>
-      <c r="D17" t="s" s="216">
-        <v>464</v>
-      </c>
-      <c r="E17" s="212">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s" s="195">
-        <v>465</v>
-      </c>
-      <c r="G17" t="s" s="195">
-        <v>466</v>
-      </c>
-      <c r="H17" t="s" s="195">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="18" ht="16" customHeight="1">
-      <c r="A18" s="211"/>
-      <c r="B18" s="212">
-        <v>13</v>
-      </c>
-      <c r="C18" s="213">
-        <v>44113</v>
-      </c>
-      <c r="D18" t="s" s="214">
-        <v>438</v>
-      </c>
-      <c r="E18" s="212">
-        <v>2.5</v>
-      </c>
-      <c r="F18" t="s" s="193">
-        <v>468</v>
-      </c>
-      <c r="G18" t="s" s="193">
-        <v>436</v>
-      </c>
       <c r="H18" t="s" s="193">
-        <v>469</v>
+        <v>494</v>
       </c>
     </row>
     <row r="19" ht="16" customHeight="1">
-      <c r="A19" s="211"/>
-      <c r="B19" s="212">
+      <c r="A19" s="212"/>
+      <c r="B19" s="213">
         <v>14</v>
       </c>
-      <c r="C19" s="213">
+      <c r="C19" s="214">
         <v>44116</v>
       </c>
-      <c r="D19" s="218"/>
-      <c r="E19" s="218"/>
+      <c r="D19" s="219"/>
+      <c r="E19" s="219"/>
       <c r="F19" s="198"/>
       <c r="G19" s="198"/>
       <c r="H19" s="198"/>
     </row>
     <row r="20" ht="16" customHeight="1">
-      <c r="A20" s="211"/>
-      <c r="B20" s="212">
+      <c r="A20" s="212"/>
+      <c r="B20" s="213">
         <v>15</v>
       </c>
-      <c r="C20" s="213">
+      <c r="C20" s="214">
         <v>44117</v>
       </c>
-      <c r="D20" t="s" s="214">
-        <v>470</v>
-      </c>
-      <c r="E20" s="212">
+      <c r="D20" t="s" s="215">
+        <v>495</v>
+      </c>
+      <c r="E20" s="213">
         <v>5</v>
       </c>
       <c r="F20" t="s" s="193">
-        <v>471</v>
+        <v>496</v>
       </c>
       <c r="G20" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H20" t="s" s="193">
-        <v>472</v>
+        <v>497</v>
       </c>
     </row>
     <row r="21" ht="16" customHeight="1">
-      <c r="A21" s="211"/>
-      <c r="B21" s="212">
+      <c r="A21" s="212"/>
+      <c r="B21" s="213">
         <v>16</v>
       </c>
-      <c r="C21" s="213">
+      <c r="C21" s="214">
         <v>44118</v>
       </c>
-      <c r="D21" s="218"/>
-      <c r="E21" s="218"/>
+      <c r="D21" s="219"/>
+      <c r="E21" s="219"/>
       <c r="F21" s="198"/>
       <c r="G21" s="198"/>
       <c r="H21" s="198"/>
     </row>
     <row r="22" ht="16" customHeight="1">
-      <c r="A22" s="211"/>
-      <c r="B22" s="212">
+      <c r="A22" s="212"/>
+      <c r="B22" s="213">
         <v>17</v>
       </c>
-      <c r="C22" s="213">
+      <c r="C22" s="214">
         <v>44119</v>
       </c>
-      <c r="D22" t="s" s="214">
-        <v>473</v>
-      </c>
-      <c r="E22" s="212">
+      <c r="D22" t="s" s="215">
+        <v>498</v>
+      </c>
+      <c r="E22" s="213">
         <v>2.5</v>
       </c>
       <c r="F22" t="s" s="193">
-        <v>474</v>
+        <v>499</v>
       </c>
       <c r="G22" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H22" t="s" s="193">
-        <v>475</v>
+        <v>500</v>
       </c>
     </row>
     <row r="23" ht="28" customHeight="1">
-      <c r="A23" s="211"/>
-      <c r="B23" s="212">
+      <c r="A23" s="212"/>
+      <c r="B23" s="213">
         <v>18</v>
       </c>
-      <c r="C23" s="213">
+      <c r="C23" s="214">
         <v>44120</v>
       </c>
-      <c r="D23" t="s" s="216">
-        <v>476</v>
-      </c>
-      <c r="E23" s="212">
+      <c r="D23" t="s" s="217">
+        <v>501</v>
+      </c>
+      <c r="E23" s="213">
         <v>4.5</v>
       </c>
       <c r="F23" t="s" s="195">
-        <v>477</v>
+        <v>502</v>
       </c>
       <c r="G23" t="s" s="195">
-        <v>478</v>
+        <v>503</v>
       </c>
       <c r="H23" t="s" s="195">
-        <v>479</v>
+        <v>504</v>
       </c>
     </row>
     <row r="24" ht="16" customHeight="1">
-      <c r="A24" s="211"/>
-      <c r="B24" s="212">
+      <c r="A24" s="212"/>
+      <c r="B24" s="213">
         <v>19</v>
       </c>
-      <c r="C24" s="213">
+      <c r="C24" s="214">
         <v>44123</v>
       </c>
-      <c r="D24" t="s" s="214">
-        <v>480</v>
-      </c>
-      <c r="E24" s="212">
+      <c r="D24" t="s" s="215">
+        <v>505</v>
+      </c>
+      <c r="E24" s="213">
         <v>1.5</v>
       </c>
       <c r="F24" t="s" s="193">
-        <v>471</v>
+        <v>496</v>
       </c>
       <c r="G24" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H24" t="s" s="193">
-        <v>472</v>
+        <v>497</v>
       </c>
     </row>
     <row r="25" ht="16" customHeight="1">
-      <c r="A25" s="211"/>
-      <c r="B25" s="212">
+      <c r="A25" s="212"/>
+      <c r="B25" s="213">
         <v>20</v>
       </c>
-      <c r="C25" s="213">
+      <c r="C25" s="214">
         <v>44124</v>
       </c>
-      <c r="D25" s="218"/>
-      <c r="E25" s="218"/>
+      <c r="D25" s="219"/>
+      <c r="E25" s="219"/>
       <c r="F25" s="198"/>
       <c r="G25" s="198"/>
       <c r="H25" s="198"/>
     </row>
     <row r="26" ht="28" customHeight="1">
-      <c r="A26" s="211"/>
-      <c r="B26" s="212">
+      <c r="A26" s="212"/>
+      <c r="B26" s="213">
         <v>21</v>
       </c>
-      <c r="C26" s="213">
+      <c r="C26" s="214">
         <v>44125</v>
       </c>
-      <c r="D26" t="s" s="216">
+      <c r="D26" t="s" s="217">
+        <v>506</v>
+      </c>
+      <c r="E26" s="213">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s" s="195">
+        <v>507</v>
+      </c>
+      <c r="G26" t="s" s="195">
         <v>481</v>
       </c>
-      <c r="E26" s="212">
-        <v>3</v>
-      </c>
-      <c r="F26" t="s" s="195">
-        <v>482</v>
-      </c>
-      <c r="G26" t="s" s="195">
-        <v>456</v>
-      </c>
       <c r="H26" t="s" s="195">
-        <v>483</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" ht="16" customHeight="1">
-      <c r="A27" s="211"/>
-      <c r="B27" s="212">
+      <c r="A27" s="212"/>
+      <c r="B27" s="213">
         <v>22</v>
       </c>
-      <c r="C27" s="213">
+      <c r="C27" s="214">
         <v>44126</v>
       </c>
-      <c r="D27" s="218"/>
-      <c r="E27" s="218"/>
+      <c r="D27" s="219"/>
+      <c r="E27" s="219"/>
       <c r="F27" s="198"/>
       <c r="G27" s="198"/>
       <c r="H27" s="198"/>
     </row>
     <row r="28" ht="28" customHeight="1">
-      <c r="A28" s="211"/>
-      <c r="B28" s="212">
+      <c r="A28" s="212"/>
+      <c r="B28" s="213">
         <v>23</v>
       </c>
-      <c r="C28" s="213">
+      <c r="C28" s="214">
         <v>44127</v>
       </c>
-      <c r="D28" t="s" s="216">
-        <v>484</v>
-      </c>
-      <c r="E28" s="212">
+      <c r="D28" t="s" s="217">
+        <v>509</v>
+      </c>
+      <c r="E28" s="213">
         <v>8</v>
       </c>
       <c r="F28" t="s" s="195">
-        <v>485</v>
+        <v>510</v>
       </c>
       <c r="G28" t="s" s="195">
-        <v>486</v>
+        <v>511</v>
       </c>
       <c r="H28" t="s" s="195">
-        <v>487</v>
+        <v>512</v>
       </c>
     </row>
     <row r="29" ht="16" customHeight="1">
-      <c r="A29" s="211"/>
-      <c r="B29" s="212">
+      <c r="A29" s="212"/>
+      <c r="B29" s="213">
         <v>24</v>
       </c>
-      <c r="C29" s="213">
+      <c r="C29" s="214">
         <v>44131</v>
       </c>
-      <c r="D29" s="218"/>
-      <c r="E29" s="218"/>
+      <c r="D29" s="219"/>
+      <c r="E29" s="219"/>
       <c r="F29" s="198"/>
       <c r="G29" s="198"/>
       <c r="H29" s="198"/>
     </row>
     <row r="30" ht="16" customHeight="1">
-      <c r="A30" s="211"/>
-      <c r="B30" s="212">
+      <c r="A30" s="212"/>
+      <c r="B30" s="213">
         <v>25</v>
       </c>
-      <c r="C30" s="213">
+      <c r="C30" s="214">
         <v>44132</v>
       </c>
-      <c r="D30" s="218"/>
-      <c r="E30" s="218"/>
+      <c r="D30" s="219"/>
+      <c r="E30" s="219"/>
       <c r="F30" s="198"/>
       <c r="G30" s="198"/>
       <c r="H30" s="198"/>
     </row>
     <row r="31" ht="16" customHeight="1">
-      <c r="A31" s="211"/>
-      <c r="B31" s="212">
+      <c r="A31" s="212"/>
+      <c r="B31" s="213">
         <v>26</v>
       </c>
-      <c r="C31" s="213">
+      <c r="C31" s="214">
         <v>44133</v>
       </c>
-      <c r="D31" t="s" s="214">
-        <v>488</v>
-      </c>
-      <c r="E31" s="212">
+      <c r="D31" t="s" s="215">
+        <v>513</v>
+      </c>
+      <c r="E31" s="213">
         <v>1</v>
       </c>
       <c r="F31" t="s" s="193">
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="G31" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H31" t="s" s="193">
-        <v>489</v>
+        <v>514</v>
       </c>
     </row>
     <row r="32" ht="16" customHeight="1">
-      <c r="A32" s="211"/>
-      <c r="B32" s="212">
+      <c r="A32" s="212"/>
+      <c r="B32" s="213">
         <v>27</v>
       </c>
-      <c r="C32" s="213">
+      <c r="C32" s="214">
         <v>44134</v>
       </c>
-      <c r="D32" t="s" s="214">
-        <v>490</v>
-      </c>
-      <c r="E32" s="212">
+      <c r="D32" t="s" s="215">
+        <v>515</v>
+      </c>
+      <c r="E32" s="213">
         <v>2</v>
       </c>
       <c r="F32" t="s" s="193">
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="G32" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H32" t="s" s="193">
-        <v>491</v>
+        <v>516</v>
       </c>
     </row>
     <row r="33" ht="28" customHeight="1">
-      <c r="A33" s="211"/>
-      <c r="B33" s="212">
+      <c r="A33" s="212"/>
+      <c r="B33" s="213">
         <v>28</v>
       </c>
-      <c r="C33" s="213">
+      <c r="C33" s="214">
         <v>44137</v>
       </c>
-      <c r="D33" t="s" s="216">
-        <v>492</v>
-      </c>
-      <c r="E33" s="212">
+      <c r="D33" t="s" s="217">
+        <v>517</v>
+      </c>
+      <c r="E33" s="213">
         <v>8</v>
       </c>
       <c r="F33" t="s" s="195">
+        <v>518</v>
+      </c>
+      <c r="G33" t="s" s="195">
+        <v>519</v>
+      </c>
+      <c r="H33" t="s" s="195">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="34" ht="16" customHeight="1">
+      <c r="A34" s="212"/>
+      <c r="B34" s="213">
+        <v>29</v>
+      </c>
+      <c r="C34" s="214">
+        <v>44138</v>
+      </c>
+      <c r="D34" t="s" s="215">
+        <v>459</v>
+      </c>
+      <c r="E34" s="213">
+        <v>8</v>
+      </c>
+      <c r="F34" t="s" s="193">
+        <v>521</v>
+      </c>
+      <c r="G34" t="s" s="193">
+        <v>522</v>
+      </c>
+      <c r="H34" t="s" s="193">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="35" ht="28" customHeight="1">
+      <c r="A35" s="212"/>
+      <c r="B35" s="213">
+        <v>30</v>
+      </c>
+      <c r="C35" s="214">
+        <v>44139</v>
+      </c>
+      <c r="D35" t="s" s="217">
+        <v>524</v>
+      </c>
+      <c r="E35" s="213">
+        <v>8</v>
+      </c>
+      <c r="F35" t="s" s="195">
+        <v>525</v>
+      </c>
+      <c r="G35" t="s" s="195">
+        <v>526</v>
+      </c>
+      <c r="H35" t="s" s="195">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="36" ht="28" customHeight="1">
+      <c r="A36" s="212"/>
+      <c r="B36" s="213">
+        <v>31</v>
+      </c>
+      <c r="C36" s="214">
+        <v>44140</v>
+      </c>
+      <c r="D36" t="s" s="217">
+        <v>528</v>
+      </c>
+      <c r="E36" s="213">
+        <v>4.5</v>
+      </c>
+      <c r="F36" t="s" s="195">
+        <v>529</v>
+      </c>
+      <c r="G36" t="s" s="195">
+        <v>481</v>
+      </c>
+      <c r="H36" t="s" s="195">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="37" ht="16" customHeight="1">
+      <c r="A37" s="212"/>
+      <c r="B37" s="213">
+        <v>32</v>
+      </c>
+      <c r="C37" s="214">
+        <v>44141</v>
+      </c>
+      <c r="D37" t="s" s="215">
+        <v>531</v>
+      </c>
+      <c r="E37" s="213">
+        <v>6.5</v>
+      </c>
+      <c r="F37" t="s" s="193">
         <v>493</v>
       </c>
-      <c r="G33" t="s" s="195">
-        <v>494</v>
-      </c>
-      <c r="H33" t="s" s="195">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="34" ht="16" customHeight="1">
-      <c r="A34" s="211"/>
-      <c r="B34" s="212">
-        <v>29</v>
-      </c>
-      <c r="C34" s="213">
-        <v>44138</v>
-      </c>
-      <c r="D34" t="s" s="214">
-        <v>434</v>
-      </c>
-      <c r="E34" s="212">
-        <v>8</v>
-      </c>
-      <c r="F34" t="s" s="193">
-        <v>496</v>
-      </c>
-      <c r="G34" t="s" s="193">
-        <v>497</v>
-      </c>
-      <c r="H34" t="s" s="193">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="35" ht="28" customHeight="1">
-      <c r="A35" s="211"/>
-      <c r="B35" s="212">
-        <v>30</v>
-      </c>
-      <c r="C35" s="213">
-        <v>44139</v>
-      </c>
-      <c r="D35" t="s" s="216">
-        <v>499</v>
-      </c>
-      <c r="E35" s="212">
-        <v>8</v>
-      </c>
-      <c r="F35" t="s" s="195">
-        <v>500</v>
-      </c>
-      <c r="G35" t="s" s="195">
-        <v>501</v>
-      </c>
-      <c r="H35" t="s" s="195">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="36" ht="28" customHeight="1">
-      <c r="A36" s="211"/>
-      <c r="B36" s="212">
-        <v>31</v>
-      </c>
-      <c r="C36" s="213">
-        <v>44140</v>
-      </c>
-      <c r="D36" t="s" s="216">
-        <v>503</v>
-      </c>
-      <c r="E36" s="212">
-        <v>4.5</v>
-      </c>
-      <c r="F36" t="s" s="195">
-        <v>504</v>
-      </c>
-      <c r="G36" t="s" s="195">
-        <v>456</v>
-      </c>
-      <c r="H36" t="s" s="195">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="37" ht="16" customHeight="1">
-      <c r="A37" s="211"/>
-      <c r="B37" s="212">
-        <v>32</v>
-      </c>
-      <c r="C37" s="213">
-        <v>44141</v>
-      </c>
-      <c r="D37" t="s" s="214">
-        <v>506</v>
-      </c>
-      <c r="E37" s="212">
-        <v>6.5</v>
-      </c>
-      <c r="F37" t="s" s="193">
-        <v>468</v>
-      </c>
       <c r="G37" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H37" t="s" s="193">
-        <v>507</v>
+        <v>532</v>
       </c>
     </row>
     <row r="38" ht="16" customHeight="1">
-      <c r="A38" s="211"/>
-      <c r="B38" s="212">
+      <c r="A38" s="212"/>
+      <c r="B38" s="213">
         <v>33</v>
       </c>
-      <c r="C38" s="213">
+      <c r="C38" s="214">
         <v>44144</v>
       </c>
-      <c r="D38" s="218"/>
-      <c r="E38" s="218"/>
+      <c r="D38" s="219"/>
+      <c r="E38" s="219"/>
       <c r="F38" s="198"/>
       <c r="G38" s="198"/>
       <c r="H38" s="198"/>
     </row>
     <row r="39" ht="16" customHeight="1">
-      <c r="A39" s="211"/>
-      <c r="B39" s="212">
+      <c r="A39" s="212"/>
+      <c r="B39" s="213">
         <v>34</v>
       </c>
-      <c r="C39" s="213">
+      <c r="C39" s="214">
         <v>44145</v>
       </c>
-      <c r="D39" t="s" s="214">
-        <v>508</v>
-      </c>
-      <c r="E39" s="212">
+      <c r="D39" t="s" s="215">
+        <v>533</v>
+      </c>
+      <c r="E39" s="213">
         <v>5</v>
       </c>
       <c r="F39" t="s" s="193">
-        <v>468</v>
+        <v>493</v>
       </c>
       <c r="G39" t="s" s="193">
-        <v>436</v>
+        <v>461</v>
       </c>
       <c r="H39" t="s" s="193">
-        <v>489</v>
+        <v>514</v>
       </c>
     </row>
     <row r="40" ht="16" customHeight="1">
-      <c r="A40" s="211"/>
-      <c r="B40" s="212">
+      <c r="A40" s="212"/>
+      <c r="B40" s="213">
         <v>35</v>
       </c>
-      <c r="C40" s="213">
+      <c r="C40" s="214">
         <v>44146</v>
       </c>
-      <c r="D40" s="218"/>
-      <c r="E40" s="218"/>
+      <c r="D40" s="219"/>
+      <c r="E40" s="219"/>
       <c r="F40" s="198"/>
       <c r="G40" s="198"/>
       <c r="H40" s="198"/>
     </row>
     <row r="41" ht="15" customHeight="1">
       <c r="A41" s="123"/>
-      <c r="B41" s="219"/>
-      <c r="C41" s="219"/>
-      <c r="D41" t="s" s="220">
-        <v>509</v>
-      </c>
-      <c r="E41" s="221">
+      <c r="B41" s="220"/>
+      <c r="C41" s="220"/>
+      <c r="D41" t="s" s="221">
+        <v>534</v>
+      </c>
+      <c r="E41" s="222">
         <f>SUM(E6:E40)</f>
         <v>140.75</v>
       </c>
-      <c r="F41" t="s" s="222">
-        <v>510</v>
-      </c>
-      <c r="G41" t="s" s="222">
+      <c r="F41" t="s" s="223">
+        <v>535</v>
+      </c>
+      <c r="G41" t="s" s="223">
         <f>"out of "&amp;8*('UAT Status'!E4-NETWORKDAYS(TODAY(),'UAT Status'!D4,'UAT Status'!$W1:$W24)+1)&amp;" hours"</f>
-        <v>511</v>
-      </c>
-      <c r="H41" s="223"/>
+        <v>536</v>
+      </c>
+      <c r="H41" s="224"/>
     </row>
     <row r="42" ht="15" customHeight="1">
       <c r="A42" s="123"/>
       <c r="B42" s="126"/>
       <c r="C42" s="126"/>
       <c r="D42" s="126"/>
-      <c r="E42" s="219"/>
+      <c r="E42" s="220"/>
       <c r="F42" s="126"/>
       <c r="G42" s="126"/>
       <c r="H42" s="127"/>
     </row>
     <row r="43" ht="16" customHeight="1">
       <c r="A43" s="174"/>
-      <c r="B43" t="s" s="224">
-        <v>512</v>
+      <c r="B43" t="s" s="225">
+        <v>537</v>
       </c>
       <c r="C43" s="187"/>
       <c r="D43" s="187"/>

</xml_diff>